<commit_message>
Revisión de escaleta guion 6
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion06/Escaleta_LE_08_06_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion06/Escaleta_LE_08_06_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luz Amparo\Documents\GitHub\Lenguaje\fuentes\contenidos\grado08\guion06\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -13,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621" iterateCount="2" iterateDelta="10"/>
 </workbook>
 </file>
 
@@ -1267,6 +1272,54 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1336,54 +1389,6 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1444,7 +1449,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1479,7 +1484,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1690,9 +1695,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U260"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H43" sqref="A43:XFD43"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="49" zoomScaleNormal="49" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1705,118 +1710,118 @@
     <col min="6" max="6" width="29.42578125" style="21" customWidth="1"/>
     <col min="7" max="7" width="46.42578125" style="3" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" style="21" customWidth="1"/>
-    <col min="9" max="9" width="11" style="61" customWidth="1"/>
+    <col min="9" max="9" width="11" style="38" customWidth="1"/>
     <col min="10" max="10" width="45.28515625" style="3" customWidth="1"/>
     <col min="11" max="11" width="20" style="3" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" style="3" customWidth="1"/>
     <col min="13" max="13" width="9.28515625" style="3" customWidth="1"/>
     <col min="14" max="14" width="11.42578125" style="3" customWidth="1"/>
     <col min="15" max="15" width="37.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="62" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="39" customWidth="1"/>
     <col min="17" max="17" width="20.42578125" style="21" customWidth="1"/>
     <col min="18" max="18" width="23" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.85546875" style="63" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21.7109375" style="3" customWidth="1"/>
     <col min="22" max="22" width="19.7109375" style="3" customWidth="1"/>
     <col min="23" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="39"/>
-      <c r="O1" s="27" t="s">
+      <c r="N1" s="55"/>
+      <c r="O1" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="46" t="s">
+      <c r="Q1" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="46" t="s">
+      <c r="R1" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="42" t="s">
+      <c r="S1" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="44" t="s">
+      <c r="T1" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="42" t="s">
+      <c r="U1" s="58" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="34"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="50"/>
       <c r="M2" s="4" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="45"/>
-      <c r="U2" s="43"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="59"/>
     </row>
     <row r="3" spans="1:21" ht="63.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -1825,34 +1830,34 @@
       <c r="D3" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="H3" s="51">
+      <c r="H3" s="28">
         <v>1</v>
       </c>
-      <c r="I3" s="51" t="s">
+      <c r="I3" s="28" t="s">
         <v>20</v>
       </c>
       <c r="J3" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="K3" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="53" t="s">
+      <c r="K3" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54" t="s">
+      <c r="M3" s="31"/>
+      <c r="N3" s="31" t="s">
         <v>45</v>
       </c>
       <c r="O3" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="P3" s="55" t="s">
+      <c r="P3" s="32" t="s">
         <v>19</v>
       </c>
       <c r="Q3" s="12">
@@ -1872,10 +1877,10 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -1884,34 +1889,34 @@
       <c r="D4" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="E4" s="49"/>
-      <c r="F4" s="50"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
       <c r="G4" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="H4" s="51">
+      <c r="H4" s="28">
         <v>2</v>
       </c>
-      <c r="I4" s="51" t="s">
+      <c r="I4" s="28" t="s">
         <v>20</v>
       </c>
       <c r="J4" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="K4" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="53" t="s">
+      <c r="K4" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54" t="s">
+      <c r="M4" s="31"/>
+      <c r="N4" s="31" t="s">
         <v>50</v>
       </c>
       <c r="O4" s="18" t="s">
         <v>293</v>
       </c>
-      <c r="P4" s="55" t="s">
+      <c r="P4" s="32" t="s">
         <v>19</v>
       </c>
       <c r="Q4" s="12">
@@ -1931,10 +1936,10 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -1948,7 +1953,7 @@
       <c r="G5" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="H5" s="51">
+      <c r="H5" s="28">
         <v>3</v>
       </c>
       <c r="I5" s="23" t="s">
@@ -1957,20 +1962,20 @@
       <c r="J5" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="K5" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="53" t="s">
+      <c r="K5" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57" t="s">
+      <c r="M5" s="34"/>
+      <c r="N5" s="34" t="s">
         <v>30</v>
       </c>
       <c r="O5" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="P5" s="55" t="s">
+      <c r="P5" s="32" t="s">
         <v>19</v>
       </c>
       <c r="Q5" s="12">
@@ -1990,10 +1995,10 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -2007,7 +2012,7 @@
       <c r="G6" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="H6" s="51">
+      <c r="H6" s="28">
         <v>4</v>
       </c>
       <c r="I6" s="23" t="s">
@@ -2016,20 +2021,20 @@
       <c r="J6" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="K6" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="53" t="s">
+      <c r="K6" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="57"/>
-      <c r="N6" s="57" t="s">
+      <c r="M6" s="34"/>
+      <c r="N6" s="34" t="s">
         <v>36</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="P6" s="55" t="s">
+      <c r="P6" s="32" t="s">
         <v>19</v>
       </c>
       <c r="Q6" s="12">
@@ -2049,10 +2054,10 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -2066,7 +2071,7 @@
       <c r="G7" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="H7" s="51">
+      <c r="H7" s="28">
         <v>5</v>
       </c>
       <c r="I7" s="23" t="s">
@@ -2075,20 +2080,20 @@
       <c r="J7" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="K7" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="53" t="s">
+      <c r="K7" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="57"/>
-      <c r="N7" s="57" t="s">
+      <c r="M7" s="34"/>
+      <c r="N7" s="34" t="s">
         <v>43</v>
       </c>
       <c r="O7" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="P7" s="55" t="s">
+      <c r="P7" s="32" t="s">
         <v>19</v>
       </c>
       <c r="Q7" s="12">
@@ -2108,10 +2113,10 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -2125,7 +2130,7 @@
       <c r="G8" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="H8" s="51">
+      <c r="H8" s="28">
         <v>6</v>
       </c>
       <c r="I8" s="23" t="s">
@@ -2134,20 +2139,20 @@
       <c r="J8" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="K8" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="53" t="s">
+      <c r="K8" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="57"/>
-      <c r="N8" s="57" t="s">
+      <c r="M8" s="34"/>
+      <c r="N8" s="34" t="s">
         <v>51</v>
       </c>
       <c r="O8" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="P8" s="55" t="s">
+      <c r="P8" s="32" t="s">
         <v>19</v>
       </c>
       <c r="Q8" s="12">
@@ -2167,10 +2172,10 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="132" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -2188,7 +2193,7 @@
       <c r="G9" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="H9" s="51">
+      <c r="H9" s="28">
         <v>7</v>
       </c>
       <c r="I9" s="23" t="s">
@@ -2197,20 +2202,20 @@
       <c r="J9" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="K9" s="56" t="s">
+      <c r="K9" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="57"/>
-      <c r="N9" s="57" t="s">
+      <c r="M9" s="34"/>
+      <c r="N9" s="34" t="s">
         <v>32</v>
       </c>
       <c r="O9" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="P9" s="58" t="s">
+      <c r="P9" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q9" s="12">
@@ -2230,10 +2235,10 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -2251,7 +2256,7 @@
       <c r="G10" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="H10" s="51">
+      <c r="H10" s="28">
         <v>8</v>
       </c>
       <c r="I10" s="23" t="s">
@@ -2260,20 +2265,20 @@
       <c r="J10" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="K10" s="56" t="s">
+      <c r="K10" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L10" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="57" t="s">
+      <c r="M10" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="N10" s="57"/>
+      <c r="N10" s="34"/>
       <c r="O10" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="P10" s="58" t="s">
+      <c r="P10" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q10" s="12">
@@ -2293,10 +2298,10 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -2314,7 +2319,7 @@
       <c r="G11" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="H11" s="51">
+      <c r="H11" s="28">
         <v>9</v>
       </c>
       <c r="I11" s="23" t="s">
@@ -2323,18 +2328,18 @@
       <c r="J11" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="K11" s="56" t="s">
+      <c r="K11" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L11" s="24"/>
-      <c r="M11" s="57"/>
-      <c r="N11" s="57" t="s">
+      <c r="M11" s="34"/>
+      <c r="N11" s="34" t="s">
         <v>24</v>
       </c>
       <c r="O11" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="P11" s="58" t="s">
+      <c r="P11" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q11" s="12">
@@ -2354,10 +2359,10 @@
       </c>
     </row>
     <row r="12" spans="1:21" ht="174" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -2375,7 +2380,7 @@
       <c r="G12" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="H12" s="51">
+      <c r="H12" s="28">
         <v>10</v>
       </c>
       <c r="I12" s="23" t="s">
@@ -2384,20 +2389,20 @@
       <c r="J12" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="K12" s="56" t="s">
+      <c r="K12" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L12" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="57" t="s">
+      <c r="M12" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="N12" s="57"/>
+      <c r="N12" s="34"/>
       <c r="O12" s="9" t="s">
         <v>328</v>
       </c>
-      <c r="P12" s="58" t="s">
+      <c r="P12" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q12" s="12">
@@ -2417,10 +2422,10 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -2438,7 +2443,7 @@
       <c r="G13" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="H13" s="51">
+      <c r="H13" s="28">
         <v>11</v>
       </c>
       <c r="I13" s="23" t="s">
@@ -2447,20 +2452,20 @@
       <c r="J13" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="K13" s="56" t="s">
+      <c r="K13" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L13" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M13" s="57"/>
-      <c r="N13" s="57" t="s">
+      <c r="M13" s="34"/>
+      <c r="N13" s="34" t="s">
         <v>31</v>
       </c>
       <c r="O13" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="P13" s="58" t="s">
+      <c r="P13" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q13" s="12">
@@ -2480,10 +2485,10 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -2501,7 +2506,7 @@
       <c r="G14" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="H14" s="51">
+      <c r="H14" s="28">
         <v>12</v>
       </c>
       <c r="I14" s="23" t="s">
@@ -2510,20 +2515,20 @@
       <c r="J14" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="K14" s="56" t="s">
+      <c r="K14" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L14" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="57"/>
-      <c r="N14" s="57" t="s">
+      <c r="M14" s="34"/>
+      <c r="N14" s="34" t="s">
         <v>33</v>
       </c>
       <c r="O14" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="P14" s="58" t="s">
+      <c r="P14" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q14" s="12">
@@ -2543,10 +2548,10 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -2562,7 +2567,7 @@
       <c r="G15" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="H15" s="51">
+      <c r="H15" s="28">
         <v>13</v>
       </c>
       <c r="I15" s="23" t="s">
@@ -2571,21 +2576,21 @@
       <c r="J15" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="K15" s="56" t="s">
+      <c r="K15" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L15" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="57"/>
-      <c r="N15" s="57" t="s">
+      <c r="M15" s="34"/>
+      <c r="N15" s="34" t="s">
         <v>121</v>
       </c>
       <c r="O15" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="P15" s="58" t="s">
-        <v>20</v>
+      <c r="P15" s="35" t="s">
+        <v>19</v>
       </c>
       <c r="Q15" s="12">
         <v>6</v>
@@ -2604,10 +2609,10 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="135" x14ac:dyDescent="0.25">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -2621,7 +2626,7 @@
       <c r="G16" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="H16" s="51">
+      <c r="H16" s="28">
         <v>14</v>
       </c>
       <c r="I16" s="23" t="s">
@@ -2630,20 +2635,20 @@
       <c r="J16" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="K16" s="56" t="s">
+      <c r="K16" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L16" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="M16" s="57" t="s">
+      <c r="M16" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="N16" s="57"/>
+      <c r="N16" s="34"/>
       <c r="O16" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="P16" s="59" t="s">
+      <c r="P16" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q16" s="12">
@@ -2663,10 +2668,10 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="120" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -2680,7 +2685,7 @@
       <c r="G17" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="H17" s="51">
+      <c r="H17" s="28">
         <v>15</v>
       </c>
       <c r="I17" s="23" t="s">
@@ -2689,18 +2694,18 @@
       <c r="J17" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="K17" s="56" t="s">
+      <c r="K17" s="33" t="s">
         <v>19</v>
       </c>
       <c r="L17" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="57"/>
-      <c r="N17" s="57"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
       <c r="O17" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="P17" s="58" t="s">
+      <c r="P17" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q17" s="12">
@@ -2720,10 +2725,10 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -2737,7 +2742,7 @@
       <c r="G18" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="H18" s="51">
+      <c r="H18" s="28">
         <v>16</v>
       </c>
       <c r="I18" s="23" t="s">
@@ -2746,18 +2751,18 @@
       <c r="J18" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="K18" s="56" t="s">
+      <c r="K18" s="33" t="s">
         <v>19</v>
       </c>
       <c r="L18" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="57"/>
-      <c r="N18" s="57"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
       <c r="O18" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="P18" s="58" t="s">
+      <c r="P18" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q18" s="12">
@@ -2777,10 +2782,10 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -2796,7 +2801,7 @@
       <c r="G19" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="H19" s="51">
+      <c r="H19" s="28">
         <v>17</v>
       </c>
       <c r="I19" s="23" t="s">
@@ -2805,18 +2810,18 @@
       <c r="J19" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="K19" s="56" t="s">
+      <c r="K19" s="33" t="s">
         <v>19</v>
       </c>
       <c r="L19" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="57"/>
-      <c r="N19" s="57"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
       <c r="O19" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="P19" s="58" t="s">
+      <c r="P19" s="35" t="s">
         <v>20</v>
       </c>
       <c r="Q19" s="12">
@@ -2836,10 +2841,10 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -2855,7 +2860,7 @@
       <c r="G20" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="H20" s="51">
+      <c r="H20" s="28">
         <v>18</v>
       </c>
       <c r="I20" s="23" t="s">
@@ -2864,20 +2869,20 @@
       <c r="J20" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="K20" s="56" t="s">
+      <c r="K20" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L20" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="57"/>
-      <c r="N20" s="57" t="s">
+      <c r="M20" s="34"/>
+      <c r="N20" s="34" t="s">
         <v>121</v>
       </c>
       <c r="O20" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="P20" s="58" t="s">
+      <c r="P20" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q20" s="12">
@@ -2897,10 +2902,10 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="105" x14ac:dyDescent="0.25">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -2916,7 +2921,7 @@
       <c r="G21" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="H21" s="51">
+      <c r="H21" s="28">
         <v>19</v>
       </c>
       <c r="I21" s="23" t="s">
@@ -2925,20 +2930,20 @@
       <c r="J21" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="K21" s="56" t="s">
+      <c r="K21" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L21" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="M21" s="57" t="s">
+      <c r="M21" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="N21" s="57"/>
+      <c r="N21" s="34"/>
       <c r="O21" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="P21" s="58" t="s">
+      <c r="P21" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q21" s="12">
@@ -2958,10 +2963,10 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="105" x14ac:dyDescent="0.25">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -2977,7 +2982,7 @@
       <c r="G22" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="H22" s="51">
+      <c r="H22" s="28">
         <v>20</v>
       </c>
       <c r="I22" s="23" t="s">
@@ -2986,20 +2991,20 @@
       <c r="J22" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="K22" s="56" t="s">
+      <c r="K22" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L22" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="57"/>
-      <c r="N22" s="57" t="s">
+      <c r="M22" s="34"/>
+      <c r="N22" s="34" t="s">
         <v>31</v>
       </c>
       <c r="O22" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="P22" s="58" t="s">
+      <c r="P22" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q22" s="12">
@@ -3019,10 +3024,10 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="48" t="s">
+      <c r="A23" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C23" s="5" t="s">
@@ -3038,7 +3043,7 @@
       <c r="G23" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="H23" s="51">
+      <c r="H23" s="28">
         <v>21</v>
       </c>
       <c r="I23" s="23" t="s">
@@ -3047,20 +3052,20 @@
       <c r="J23" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="K23" s="56" t="s">
+      <c r="K23" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L23" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="57"/>
-      <c r="N23" s="57" t="s">
+      <c r="M23" s="34"/>
+      <c r="N23" s="34" t="s">
         <v>121</v>
       </c>
       <c r="O23" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="P23" s="58" t="s">
+      <c r="P23" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q23" s="12">
@@ -3080,10 +3085,10 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -3099,7 +3104,7 @@
       <c r="G24" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="H24" s="51">
+      <c r="H24" s="28">
         <v>22</v>
       </c>
       <c r="I24" s="23" t="s">
@@ -3108,18 +3113,18 @@
       <c r="J24" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="K24" s="56" t="s">
+      <c r="K24" s="33" t="s">
         <v>19</v>
       </c>
       <c r="L24" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M24" s="57"/>
-      <c r="N24" s="57"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
       <c r="O24" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="P24" s="59" t="s">
+      <c r="P24" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q24" s="12">
@@ -3139,10 +3144,10 @@
       </c>
     </row>
     <row r="25" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -3160,7 +3165,7 @@
       <c r="G25" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="H25" s="51">
+      <c r="H25" s="28">
         <v>23</v>
       </c>
       <c r="I25" s="23" t="s">
@@ -3169,20 +3174,20 @@
       <c r="J25" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="K25" s="56" t="s">
+      <c r="K25" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L25" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M25" s="57"/>
-      <c r="N25" s="57" t="s">
+      <c r="M25" s="34"/>
+      <c r="N25" s="34" t="s">
         <v>24</v>
       </c>
       <c r="O25" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="P25" s="59" t="s">
+      <c r="P25" s="36" t="s">
         <v>20</v>
       </c>
       <c r="Q25" s="12">
@@ -3202,10 +3207,10 @@
       </c>
     </row>
     <row r="26" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" s="48" t="s">
+      <c r="A26" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -3223,7 +3228,7 @@
       <c r="G26" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="H26" s="51">
+      <c r="H26" s="28">
         <v>24</v>
       </c>
       <c r="I26" s="23" t="s">
@@ -3232,20 +3237,20 @@
       <c r="J26" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="K26" s="56" t="s">
+      <c r="K26" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L26" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="M26" s="57" t="s">
+      <c r="M26" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="N26" s="57"/>
+      <c r="N26" s="34"/>
       <c r="O26" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="P26" s="59" t="s">
+      <c r="P26" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q26" s="12">
@@ -3265,10 +3270,10 @@
       </c>
     </row>
     <row r="27" spans="1:21" ht="135" x14ac:dyDescent="0.25">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -3286,7 +3291,7 @@
       <c r="G27" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="H27" s="51">
+      <c r="H27" s="28">
         <v>25</v>
       </c>
       <c r="I27" s="23" t="s">
@@ -3295,18 +3300,18 @@
       <c r="J27" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="K27" s="56" t="s">
+      <c r="K27" s="33" t="s">
         <v>19</v>
       </c>
       <c r="L27" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M27" s="57"/>
-      <c r="N27" s="57"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="34"/>
       <c r="O27" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="P27" s="59" t="s">
+      <c r="P27" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q27" s="12">
@@ -3326,10 +3331,10 @@
       </c>
     </row>
     <row r="28" spans="1:21" ht="135" x14ac:dyDescent="0.25">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C28" s="5" t="s">
@@ -3347,7 +3352,7 @@
       <c r="G28" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="H28" s="51">
+      <c r="H28" s="28">
         <v>26</v>
       </c>
       <c r="I28" s="23" t="s">
@@ -3356,20 +3361,20 @@
       <c r="J28" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="K28" s="56" t="s">
+      <c r="K28" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L28" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="57"/>
-      <c r="N28" s="57" t="s">
+      <c r="M28" s="34"/>
+      <c r="N28" s="34" t="s">
         <v>45</v>
       </c>
       <c r="O28" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="P28" s="59" t="s">
+      <c r="P28" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q28" s="12">
@@ -3389,10 +3394,10 @@
       </c>
     </row>
     <row r="29" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="49" t="s">
+      <c r="B29" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -3410,7 +3415,7 @@
       <c r="G29" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="H29" s="51">
+      <c r="H29" s="28">
         <v>27</v>
       </c>
       <c r="I29" s="23" t="s">
@@ -3419,20 +3424,20 @@
       <c r="J29" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="K29" s="56" t="s">
+      <c r="K29" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L29" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="M29" s="57" t="s">
+      <c r="M29" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="N29" s="57"/>
+      <c r="N29" s="34"/>
       <c r="O29" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="P29" s="59" t="s">
+      <c r="P29" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q29" s="12">
@@ -3452,8 +3457,8 @@
       </c>
     </row>
     <row r="30" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="48"/>
-      <c r="B30" s="49"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="5" t="s">
         <v>150</v>
       </c>
@@ -3467,7 +3472,7 @@
       <c r="G30" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="H30" s="51">
+      <c r="H30" s="28">
         <v>28</v>
       </c>
       <c r="I30" s="23" t="s">
@@ -3476,20 +3481,20 @@
       <c r="J30" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="K30" s="56" t="s">
+      <c r="K30" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L30" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M30" s="57"/>
-      <c r="N30" s="57" t="s">
+      <c r="M30" s="34"/>
+      <c r="N30" s="34" t="s">
         <v>30</v>
       </c>
       <c r="O30" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="P30" s="59" t="s">
+      <c r="P30" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q30" s="12">
@@ -3509,10 +3514,10 @@
       </c>
     </row>
     <row r="31" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="49" t="s">
+      <c r="B31" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C31" s="5" t="s">
@@ -3528,7 +3533,7 @@
       <c r="G31" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="H31" s="51">
+      <c r="H31" s="28">
         <v>29</v>
       </c>
       <c r="I31" s="23" t="s">
@@ -3537,18 +3542,18 @@
       <c r="J31" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="K31" s="56" t="s">
+      <c r="K31" s="33" t="s">
         <v>19</v>
       </c>
       <c r="L31" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M31" s="57"/>
-      <c r="N31" s="57"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="34"/>
       <c r="O31" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="P31" s="59" t="s">
+      <c r="P31" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q31" s="12">
@@ -3568,8 +3573,8 @@
       </c>
     </row>
     <row r="32" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
-      <c r="B32" s="49"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="26"/>
       <c r="C32" s="5" t="s">
         <v>150</v>
       </c>
@@ -3583,7 +3588,7 @@
       <c r="G32" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="H32" s="51">
+      <c r="H32" s="28">
         <v>30</v>
       </c>
       <c r="I32" s="23" t="s">
@@ -3592,18 +3597,18 @@
       <c r="J32" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="K32" s="56" t="s">
+      <c r="K32" s="33" t="s">
         <v>19</v>
       </c>
       <c r="L32" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M32" s="57"/>
-      <c r="N32" s="57"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="34"/>
       <c r="O32" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="P32" s="59" t="s">
+      <c r="P32" s="36" t="s">
         <v>20</v>
       </c>
       <c r="Q32" s="12">
@@ -3623,10 +3628,10 @@
       </c>
     </row>
     <row r="33" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="48" t="s">
+      <c r="A33" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C33" s="5" t="s">
@@ -3642,7 +3647,7 @@
       <c r="G33" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="H33" s="51">
+      <c r="H33" s="28">
         <v>31</v>
       </c>
       <c r="I33" s="23" t="s">
@@ -3651,19 +3656,19 @@
       <c r="J33" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="K33" s="56" t="s">
+      <c r="K33" s="33" t="s">
         <v>19</v>
       </c>
       <c r="L33" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M33" s="57"/>
-      <c r="N33" s="57"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="34"/>
       <c r="O33" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="P33" s="59" t="s">
-        <v>20</v>
+      <c r="P33" s="36" t="s">
+        <v>19</v>
       </c>
       <c r="Q33" s="12">
         <v>10</v>
@@ -3682,10 +3687,10 @@
       </c>
     </row>
     <row r="34" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="48" t="s">
+      <c r="A34" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C34" s="5" t="s">
@@ -3699,7 +3704,7 @@
       <c r="G34" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="H34" s="51">
+      <c r="H34" s="28">
         <v>32</v>
       </c>
       <c r="I34" s="23" t="s">
@@ -3708,20 +3713,20 @@
       <c r="J34" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="K34" s="56" t="s">
+      <c r="K34" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L34" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="M34" s="57" t="s">
+      <c r="M34" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="N34" s="57"/>
+      <c r="N34" s="34"/>
       <c r="O34" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="P34" s="59" t="s">
+      <c r="P34" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q34" s="12">
@@ -3741,10 +3746,10 @@
       </c>
     </row>
     <row r="35" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="48" t="s">
+      <c r="A35" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -3758,7 +3763,7 @@
       <c r="G35" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="H35" s="51">
+      <c r="H35" s="28">
         <v>33</v>
       </c>
       <c r="I35" s="23" t="s">
@@ -3767,18 +3772,18 @@
       <c r="J35" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="K35" s="56" t="s">
+      <c r="K35" s="33" t="s">
         <v>19</v>
       </c>
       <c r="L35" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M35" s="57"/>
-      <c r="N35" s="57"/>
+      <c r="M35" s="34"/>
+      <c r="N35" s="34"/>
       <c r="O35" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="P35" s="59" t="s">
+      <c r="P35" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q35" s="12">
@@ -3798,10 +3803,10 @@
       </c>
     </row>
     <row r="36" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C36" s="5" t="s">
@@ -3817,7 +3822,7 @@
       <c r="G36" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="H36" s="51">
+      <c r="H36" s="28">
         <v>34</v>
       </c>
       <c r="I36" s="23" t="s">
@@ -3826,18 +3831,18 @@
       <c r="J36" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="K36" s="56" t="s">
+      <c r="K36" s="33" t="s">
         <v>19</v>
       </c>
       <c r="L36" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M36" s="57"/>
-      <c r="N36" s="57"/>
+      <c r="M36" s="34"/>
+      <c r="N36" s="34"/>
       <c r="O36" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="P36" s="59" t="s">
+      <c r="P36" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q36" s="12">
@@ -3857,10 +3862,10 @@
       </c>
     </row>
     <row r="37" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="49" t="s">
+      <c r="B37" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C37" s="5" t="s">
@@ -3876,7 +3881,7 @@
       <c r="G37" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="H37" s="51">
+      <c r="H37" s="28">
         <v>35</v>
       </c>
       <c r="I37" s="23" t="s">
@@ -3885,20 +3890,20 @@
       <c r="J37" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="K37" s="56" t="s">
+      <c r="K37" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L37" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M37" s="57"/>
-      <c r="N37" s="57" t="s">
+      <c r="M37" s="34"/>
+      <c r="N37" s="34" t="s">
         <v>121</v>
       </c>
       <c r="O37" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="P37" s="59" t="s">
+      <c r="P37" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q37" s="12">
@@ -3918,10 +3923,10 @@
       </c>
     </row>
     <row r="38" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A38" s="48" t="s">
+      <c r="A38" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -3932,10 +3937,10 @@
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="9"/>
-      <c r="G38" s="60" t="s">
+      <c r="G38" s="37" t="s">
         <v>281</v>
       </c>
-      <c r="H38" s="51">
+      <c r="H38" s="28">
         <v>36</v>
       </c>
       <c r="I38" s="23" t="s">
@@ -3944,21 +3949,21 @@
       <c r="J38" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="K38" s="56" t="s">
+      <c r="K38" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L38" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M38" s="57"/>
-      <c r="N38" s="57" t="s">
+      <c r="M38" s="34"/>
+      <c r="N38" s="34" t="s">
         <v>28</v>
       </c>
       <c r="O38" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="P38" s="59" t="s">
-        <v>20</v>
+      <c r="P38" s="36" t="s">
+        <v>19</v>
       </c>
       <c r="Q38" s="12">
         <v>6</v>
@@ -3977,10 +3982,10 @@
       </c>
     </row>
     <row r="39" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="48" t="s">
+      <c r="A39" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="49" t="s">
+      <c r="B39" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -3994,7 +3999,7 @@
       <c r="G39" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="H39" s="51">
+      <c r="H39" s="28">
         <v>37</v>
       </c>
       <c r="I39" s="23" t="s">
@@ -4003,21 +4008,21 @@
       <c r="J39" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K39" s="56" t="s">
+      <c r="K39" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L39" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M39" s="57"/>
-      <c r="N39" s="57" t="s">
+      <c r="M39" s="34"/>
+      <c r="N39" s="34" t="s">
         <v>35</v>
       </c>
       <c r="O39" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="P39" s="59" t="s">
-        <v>20</v>
+      <c r="P39" s="36" t="s">
+        <v>19</v>
       </c>
       <c r="Q39" s="12">
         <v>6</v>
@@ -4036,10 +4041,10 @@
       </c>
     </row>
     <row r="40" spans="1:21" ht="105" x14ac:dyDescent="0.25">
-      <c r="A40" s="48" t="s">
+      <c r="A40" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="49" t="s">
+      <c r="B40" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -4053,7 +4058,7 @@
       <c r="G40" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="H40" s="51">
+      <c r="H40" s="28">
         <v>38</v>
       </c>
       <c r="I40" s="23" t="s">
@@ -4062,21 +4067,21 @@
       <c r="J40" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="K40" s="56" t="s">
+      <c r="K40" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L40" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M40" s="57"/>
-      <c r="N40" s="57" t="s">
+      <c r="M40" s="34"/>
+      <c r="N40" s="34" t="s">
         <v>36</v>
       </c>
       <c r="O40" s="9" t="s">
         <v>323</v>
       </c>
-      <c r="P40" s="59" t="s">
-        <v>20</v>
+      <c r="P40" s="36" t="s">
+        <v>19</v>
       </c>
       <c r="Q40" s="12">
         <v>6</v>
@@ -4095,10 +4100,10 @@
       </c>
     </row>
     <row r="41" spans="1:21" ht="165" x14ac:dyDescent="0.25">
-      <c r="A41" s="48" t="s">
+      <c r="A41" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B41" s="49" t="s">
+      <c r="B41" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -4112,7 +4117,7 @@
       <c r="G41" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="H41" s="51">
+      <c r="H41" s="28">
         <v>39</v>
       </c>
       <c r="I41" s="23" t="s">
@@ -4121,20 +4126,20 @@
       <c r="J41" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="K41" s="56" t="s">
+      <c r="K41" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L41" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="M41" s="57" t="s">
+      <c r="M41" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="N41" s="57"/>
+      <c r="N41" s="34"/>
       <c r="O41" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="P41" s="59" t="s">
+      <c r="P41" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q41" s="12">
@@ -4154,10 +4159,10 @@
       </c>
     </row>
     <row r="42" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="49" t="s">
+      <c r="B42" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -4171,7 +4176,7 @@
       <c r="G42" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H42" s="51">
+      <c r="H42" s="28">
         <v>40</v>
       </c>
       <c r="I42" s="23" t="s">
@@ -4180,18 +4185,18 @@
       <c r="J42" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="K42" s="56" t="s">
+      <c r="K42" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L42" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="M42" s="57"/>
-      <c r="N42" s="57"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="34"/>
       <c r="O42" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="P42" s="59" t="s">
+      <c r="P42" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q42" s="12"/>
@@ -4201,10 +4206,10 @@
       <c r="U42" s="12"/>
     </row>
     <row r="43" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="48" t="s">
+      <c r="A43" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B43" s="49" t="s">
+      <c r="B43" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C43" s="5" t="s">
@@ -4218,7 +4223,7 @@
       <c r="G43" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="H43" s="51">
+      <c r="H43" s="28">
         <v>41</v>
       </c>
       <c r="I43" s="23" t="s">
@@ -4227,20 +4232,20 @@
       <c r="J43" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="K43" s="56" t="s">
+      <c r="K43" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L43" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M43" s="57"/>
-      <c r="N43" s="57" t="s">
+      <c r="M43" s="34"/>
+      <c r="N43" s="34" t="s">
         <v>32</v>
       </c>
       <c r="O43" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="P43" s="59" t="s">
+      <c r="P43" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q43" s="12">
@@ -4260,10 +4265,10 @@
       </c>
     </row>
     <row r="44" spans="1:21" ht="105" x14ac:dyDescent="0.25">
-      <c r="A44" s="48" t="s">
+      <c r="A44" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B44" s="49" t="s">
+      <c r="B44" s="26" t="s">
         <v>122</v>
       </c>
       <c r="C44" s="5" t="s">
@@ -4277,7 +4282,7 @@
       <c r="G44" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="H44" s="51">
+      <c r="H44" s="28">
         <v>42</v>
       </c>
       <c r="I44" s="23" t="s">
@@ -4286,20 +4291,20 @@
       <c r="J44" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="K44" s="56" t="s">
+      <c r="K44" s="33" t="s">
         <v>20</v>
       </c>
       <c r="L44" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M44" s="57"/>
-      <c r="N44" s="57" t="s">
+      <c r="M44" s="34"/>
+      <c r="N44" s="34" t="s">
         <v>52</v>
       </c>
       <c r="O44" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="P44" s="59" t="s">
+      <c r="P44" s="36" t="s">
         <v>19</v>
       </c>
       <c r="Q44" s="12">

</xml_diff>